<commit_message>
more configuration (category, conditions)
</commit_message>
<xml_diff>
--- a/src/test/resources/net/enanomapper/parser/csv/ProteinCoronaTest1.xlsx
+++ b/src/test/resources/net/enanomapper/parser/csv/ProteinCoronaTest1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6952" uniqueCount="2430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6940" uniqueCount="2431">
   <si>
     <t>EndpointCategory</t>
   </si>
@@ -7304,6 +7304,9 @@
   </si>
   <si>
     <t>Cationic</t>
+  </si>
+  <si>
+    <t>Tecnai 20 (FEI) microscope;AMT 16000 camera</t>
   </si>
 </sst>
 </file>
@@ -8135,7 +8138,7 @@
   <dimension ref="A1:AGL14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10711,15 +10714,6 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
       <c r="P2" t="s">
         <v>12</v>
       </c>
@@ -13314,15 +13308,6 @@
       <c r="L3" t="s">
         <v>835</v>
       </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
       <c r="P3" t="s">
         <v>18</v>
       </c>
@@ -15922,15 +15907,6 @@
       <c r="L5" t="s">
         <v>11</v>
       </c>
-      <c r="M5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" t="s">
-        <v>11</v>
-      </c>
       <c r="P5" t="s">
         <v>12</v>
       </c>
@@ -18523,16 +18499,7 @@
         <v>835</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" t="s">
-        <v>26</v>
+        <v>2430</v>
       </c>
       <c r="P6" t="s">
         <v>27</v>

</xml_diff>